<commit_message>
With 8/11 successfully calculated red flags.
</commit_message>
<xml_diff>
--- a/data/cached_generated_reports/2024-2025/red_flag_10.xlsx
+++ b/data/cached_generated_reports/2024-2025/red_flag_10.xlsx
@@ -511,12 +511,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>6900018000</t>
+          <t>3100785000000J</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BROADBAND SYSTEMS CORPORATION  LTD</t>
+          <t>INTERSEC SECURITY COMPANY  LTD ISCO</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -526,27 +526,27 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>BROADBAND SYSTEMS CORPORATION  LTD</t>
+          <t>INTERSEC SECURITY COMPANY  LTD ISCO</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
+          <t>Kanogo Gikondo Kicukiro</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
+          <t>Kanogo Gikondo Kicukiro</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
+          <t>Kanogo Gikondo Kicukiro</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>7229 KIGALI, RWANDA</t>
+          <t>2146</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -556,22 +556,22 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>gilbert.kayinamura@bsc.rw</t>
+          <t>dnyangezi@isco.co.rw</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>4141</t>
+          <t>0788310020</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>www.bsc.rw</t>
+          <t>www.isco.co.rw</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>1198080006094070</t>
+          <t>1198770170398131</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -586,19 +586,19 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>101982714</t>
+          <t>100076965</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>6900018000</t>
+          <t>3100989200000S</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>INYANGE INDUSTRIES  LTD</t>
+          <t>H.VEDASTE COMPANY Ltd</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -608,27 +608,27 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>INYANGE INDUSTRIES  LTD</t>
+          <t>H.VEDASTE COMPANY Ltd</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>MASAKA GASABO DISTRICT</t>
+          <t>Kicukiro/Kigali</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>MASAKA GASABO DISTRICT</t>
+          <t>Kicukiro/Kigali</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>MASAKA GASABO DISTRICT</t>
+          <t>Kicukiro/Kigali</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>4584 kigali-rwanda</t>
+          <t>25 NGOMA</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -638,49 +638,44 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>bjames@inyangeindustries.com</t>
+          <t>hitimanaveda16@gmail.com</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0788309662</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>www.inyangeindustries.com</t>
+          <t>0788562686</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>1197580006310064</t>
+          <t>1196280064731068</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Rwandan</t>
+          <t>RWANDA</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>NCBA</t>
+          <t>BPR</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>100095380</t>
+          <t>115405774</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>6900018000</t>
+          <t>3102226900000M</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>H.VEDASTE COMPANY Ltd</t>
+          <t>BROADBAND SYSTEMS CORPORATION  LTD</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -690,27 +685,27 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>H.VEDASTE COMPANY Ltd</t>
+          <t>BROADBAND SYSTEMS CORPORATION  LTD</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Kicukiro/Kigali</t>
+          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Kicukiro/Kigali</t>
+          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Kicukiro/Kigali</t>
+          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>25 NGOMA</t>
+          <t>7229 KIGALI, RWANDA</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -720,17 +715,22 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>hitimanaveda16@gmail.com</t>
+          <t>gilbert.kayinamura@bsc.rw</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>0788562686</t>
+          <t>4141</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>www.bsc.rw</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>1196280064731068</t>
+          <t>1198080006094070</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -740,24 +740,24 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>BPR</t>
+          <t>BK</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>115405774</t>
+          <t>101982714</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>6900018000</t>
+          <t>3109596400000L</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>INTERSEC SECURITY COMPANY  LTD ISCO</t>
+          <t>NEPOMSCENE BUSINESS COMPANY  LTD</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -767,27 +767,22 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>INTERSEC SECURITY COMPANY  LTD ISCO</t>
+          <t>NEPOMSCENE BUSINESS COMPANY  LTD</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Kanogo Gikondo Kicukiro</t>
+          <t>NYAMAGABE District,Gasaka Sector</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Kanogo Gikondo Kicukiro</t>
+          <t>NYAMAGABE District,Gasaka Sector</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Kanogo Gikondo Kicukiro</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>2146</t>
+          <t>NYAMAGABE District,Gasaka Sector</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -797,22 +792,17 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>dnyangezi@isco.co.rw</t>
+          <t>nbchvgmn@gmail.com</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0788310020</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>www.isco.co.rw</t>
+          <t>0788475217</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>1198770170398131</t>
+          <t>1198380172943184</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -822,19 +812,19 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>BK</t>
+          <t>EQUITY BANK</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>100076965</t>
+          <t>103496546</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>6900018000</t>
+          <t>3100580400000V</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -911,12 +901,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>6900018000</t>
+          <t>3100960800000N</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CONNECT GLOBAL BUSINESS COMPANY Ltd</t>
+          <t>INYANGE INDUSTRIES  LTD</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -926,27 +916,27 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CONNECT GLOBAL BUSINESS COMPANY Ltd</t>
+          <t>INYANGE INDUSTRIES  LTD</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>KIGALI - NYARUGENGE</t>
+          <t>MASAKA GASABO DISTRICT</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>KIGALI - NYARUGENGE</t>
+          <t>MASAKA GASABO DISTRICT</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>KIGALI - NYARUGENGE</t>
+          <t>MASAKA GASABO DISTRICT</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>POB:5564 Kigali</t>
+          <t>4584 kigali-rwanda</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -956,44 +946,49 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>niyafeos@yahoo.fr</t>
+          <t>bjames@inyangeindustries.com</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>788757320</t>
+          <t>0788309662</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>www.inyangeindustries.com</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>1197980004514176</t>
+          <t>1197580006310064</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>RWANDA</t>
+          <t>Rwandan</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>I&amp;M Bank</t>
+          <t>NCBA</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>106907027</t>
+          <t>100095380</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>6900018000</t>
+          <t>3114072400000X</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>NEPOMSCENE BUSINESS COMPANY  LTD</t>
+          <t>CONNECT GLOBAL BUSINESS COMPANY Ltd</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1003,22 +998,27 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>NEPOMSCENE BUSINESS COMPANY  LTD</t>
+          <t>CONNECT GLOBAL BUSINESS COMPANY Ltd</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>NYAMAGABE District,Gasaka Sector</t>
+          <t>KIGALI - NYARUGENGE</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>NYAMAGABE District,Gasaka Sector</t>
+          <t>KIGALI - NYARUGENGE</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>NYAMAGABE District,Gasaka Sector</t>
+          <t>KIGALI - NYARUGENGE</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>POB:5564 Kigali</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1028,17 +1028,17 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>nbchvgmn@gmail.com</t>
+          <t>niyafeos@yahoo.fr</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>0788475217</t>
+          <t>788757320</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>1198380172943184</t>
+          <t>1197980004514176</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
@@ -1048,12 +1048,12 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>EQUITY BANK</t>
+          <t>I&amp;M Bank</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>103496546</t>
+          <t>106907027</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
All red flags except those without data, 2 in particular
</commit_message>
<xml_diff>
--- a/data/cached_generated_reports/2024-2025/red_flag_10.xlsx
+++ b/data/cached_generated_reports/2024-2025/red_flag_10.xlsx
@@ -511,12 +511,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>3100785000000J</t>
+          <t>3100580400000V</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>INTERSEC SECURITY COMPANY  LTD ISCO</t>
+          <t>SOCIETE RWANDAISE DES PNEUMATIQUES BANDAG  LTD</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -526,27 +526,27 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>INTERSEC SECURITY COMPANY  LTD ISCO</t>
+          <t>SOCIETE RWANDAISE DES PNEUMATIQUES BANDAG  LTD</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Kanogo Gikondo Kicukiro</t>
+          <t>Kicukiro- Rwanda</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Kanogo Gikondo Kicukiro</t>
+          <t>Kicukiro- Rwanda</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Kanogo Gikondo Kicukiro</t>
+          <t>Kicukiro- Rwanda</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2146</t>
+          <t>1132 kigali</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -556,37 +556,32 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>dnyangezi@isco.co.rw</t>
+          <t>bandag@subizo.com</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0788310020</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>www.isco.co.rw</t>
+          <t>0788303361</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>1198770170398131</t>
+          <t>AA3035975</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>RWANDA</t>
+          <t>ITALY</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>BK</t>
+          <t>I&amp;M Bank</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>100076965</t>
+          <t>100003368</t>
         </is>
       </c>
     </row>
@@ -670,12 +665,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3102226900000M</t>
+          <t>3100960800000N</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BROADBAND SYSTEMS CORPORATION  LTD</t>
+          <t>INYANGE INDUSTRIES  LTD</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -685,27 +680,27 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>BROADBAND SYSTEMS CORPORATION  LTD</t>
+          <t>INYANGE INDUSTRIES  LTD</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
+          <t>MASAKA GASABO DISTRICT</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
+          <t>MASAKA GASABO DISTRICT</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
+          <t>MASAKA GASABO DISTRICT</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>7229 KIGALI, RWANDA</t>
+          <t>4584 kigali-rwanda</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -715,49 +710,49 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>gilbert.kayinamura@bsc.rw</t>
+          <t>bjames@inyangeindustries.com</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>4141</t>
+          <t>0788309662</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>www.bsc.rw</t>
+          <t>www.inyangeindustries.com</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>1198080006094070</t>
+          <t>1197580006310064</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>RWANDA</t>
+          <t>Rwandan</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>BK</t>
+          <t>NCBA</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>101982714</t>
+          <t>100095380</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3109596400000L</t>
+          <t>3102226900000M</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>NEPOMSCENE BUSINESS COMPANY  LTD</t>
+          <t>BROADBAND SYSTEMS CORPORATION  LTD</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -767,22 +762,27 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>NEPOMSCENE BUSINESS COMPANY  LTD</t>
+          <t>BROADBAND SYSTEMS CORPORATION  LTD</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>NYAMAGABE District,Gasaka Sector</t>
+          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>NYAMAGABE District,Gasaka Sector</t>
+          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>NYAMAGABE District,Gasaka Sector</t>
+          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>7229 KIGALI, RWANDA</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -792,17 +792,22 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>nbchvgmn@gmail.com</t>
+          <t>gilbert.kayinamura@bsc.rw</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0788475217</t>
+          <t>4141</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>www.bsc.rw</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>1198380172943184</t>
+          <t>1198080006094070</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -812,24 +817,24 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>EQUITY BANK</t>
+          <t>BK</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>103496546</t>
+          <t>101982714</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3100580400000V</t>
+          <t>3114072400000X</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SOCIETE RWANDAISE DES PNEUMATIQUES BANDAG  LTD</t>
+          <t>CONNECT GLOBAL BUSINESS COMPANY Ltd</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -839,27 +844,27 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>SOCIETE RWANDAISE DES PNEUMATIQUES BANDAG  LTD</t>
+          <t>CONNECT GLOBAL BUSINESS COMPANY Ltd</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Kicukiro- Rwanda</t>
+          <t>KIGALI - NYARUGENGE</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Kicukiro- Rwanda</t>
+          <t>KIGALI - NYARUGENGE</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Kicukiro- Rwanda</t>
+          <t>KIGALI - NYARUGENGE</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>1132 kigali</t>
+          <t>POB:5564 Kigali</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -869,22 +874,22 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>bandag@subizo.com</t>
+          <t>niyafeos@yahoo.fr</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>0788303361</t>
+          <t>788757320</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>AA3035975</t>
+          <t>1197980004514176</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>ITALY</t>
+          <t>RWANDA</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -894,19 +899,19 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>100003368</t>
+          <t>106907027</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>3100960800000N</t>
+          <t>3100785000000J</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>INYANGE INDUSTRIES  LTD</t>
+          <t>INTERSEC SECURITY COMPANY  LTD ISCO</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -916,27 +921,27 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>INYANGE INDUSTRIES  LTD</t>
+          <t>INTERSEC SECURITY COMPANY  LTD ISCO</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>MASAKA GASABO DISTRICT</t>
+          <t>Kanogo Gikondo Kicukiro</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>MASAKA GASABO DISTRICT</t>
+          <t>Kanogo Gikondo Kicukiro</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>MASAKA GASABO DISTRICT</t>
+          <t>Kanogo Gikondo Kicukiro</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>4584 kigali-rwanda</t>
+          <t>2146</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -946,49 +951,49 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>bjames@inyangeindustries.com</t>
+          <t>dnyangezi@isco.co.rw</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>0788309662</t>
+          <t>0788310020</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>www.inyangeindustries.com</t>
+          <t>www.isco.co.rw</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>1197580006310064</t>
+          <t>1198770170398131</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Rwandan</t>
+          <t>RWANDA</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>NCBA</t>
+          <t>BK</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>100095380</t>
+          <t>100076965</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>3114072400000X</t>
+          <t>3109596400000L</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CONNECT GLOBAL BUSINESS COMPANY Ltd</t>
+          <t>NEPOMSCENE BUSINESS COMPANY  LTD</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -998,27 +1003,22 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>CONNECT GLOBAL BUSINESS COMPANY Ltd</t>
+          <t>NEPOMSCENE BUSINESS COMPANY  LTD</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>KIGALI - NYARUGENGE</t>
+          <t>NYAMAGABE District,Gasaka Sector</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>KIGALI - NYARUGENGE</t>
+          <t>NYAMAGABE District,Gasaka Sector</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>KIGALI - NYARUGENGE</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>POB:5564 Kigali</t>
+          <t>NYAMAGABE District,Gasaka Sector</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1028,17 +1028,17 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>niyafeos@yahoo.fr</t>
+          <t>nbchvgmn@gmail.com</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>788757320</t>
+          <t>0788475217</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>1197980004514176</t>
+          <t>1198380172943184</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
@@ -1048,12 +1048,12 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>I&amp;M Bank</t>
+          <t>EQUITY BANK</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>106907027</t>
+          <t>103496546</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Starting to include tabulated data
</commit_message>
<xml_diff>
--- a/data/cached_generated_reports/2024-2025/red_flag_10.xlsx
+++ b/data/cached_generated_reports/2024-2025/red_flag_10.xlsx
@@ -511,12 +511,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>3100580400000V</t>
+          <t>3114072400000X</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SOCIETE RWANDAISE DES PNEUMATIQUES BANDAG  LTD</t>
+          <t>CONNECT GLOBAL BUSINESS COMPANY Ltd</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -526,27 +526,27 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>SOCIETE RWANDAISE DES PNEUMATIQUES BANDAG  LTD</t>
+          <t>CONNECT GLOBAL BUSINESS COMPANY Ltd</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Kicukiro- Rwanda</t>
+          <t>KIGALI - NYARUGENGE</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Kicukiro- Rwanda</t>
+          <t>KIGALI - NYARUGENGE</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Kicukiro- Rwanda</t>
+          <t>KIGALI - NYARUGENGE</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1132 kigali</t>
+          <t>POB:5564 Kigali</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -556,22 +556,22 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>bandag@subizo.com</t>
+          <t>niyafeos@yahoo.fr</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0788303361</t>
+          <t>788757320</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>AA3035975</t>
+          <t>1197980004514176</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>ITALY</t>
+          <t>RWANDA</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -581,19 +581,19 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>100003368</t>
+          <t>106907027</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3100989200000S</t>
+          <t>3100580400000V</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>H.VEDASTE COMPANY Ltd</t>
+          <t>SOCIETE RWANDAISE DES PNEUMATIQUES BANDAG  LTD</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -603,27 +603,27 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>H.VEDASTE COMPANY Ltd</t>
+          <t>SOCIETE RWANDAISE DES PNEUMATIQUES BANDAG  LTD</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Kicukiro/Kigali</t>
+          <t>Kicukiro- Rwanda</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Kicukiro/Kigali</t>
+          <t>Kicukiro- Rwanda</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Kicukiro/Kigali</t>
+          <t>Kicukiro- Rwanda</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>25 NGOMA</t>
+          <t>1132 kigali</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -633,44 +633,44 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>hitimanaveda16@gmail.com</t>
+          <t>bandag@subizo.com</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0788562686</t>
+          <t>0788303361</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>1196280064731068</t>
+          <t>AA3035975</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>RWANDA</t>
+          <t>ITALY</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>BPR</t>
+          <t>I&amp;M Bank</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>115405774</t>
+          <t>100003368</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3100960800000N</t>
+          <t>3109596400000L</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>INYANGE INDUSTRIES  LTD</t>
+          <t>NEPOMSCENE BUSINESS COMPANY  LTD</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -680,27 +680,22 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>INYANGE INDUSTRIES  LTD</t>
+          <t>NEPOMSCENE BUSINESS COMPANY  LTD</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>MASAKA GASABO DISTRICT</t>
+          <t>NYAMAGABE District,Gasaka Sector</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>MASAKA GASABO DISTRICT</t>
+          <t>NYAMAGABE District,Gasaka Sector</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>MASAKA GASABO DISTRICT</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>4584 kigali-rwanda</t>
+          <t>NYAMAGABE District,Gasaka Sector</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -710,49 +705,44 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>bjames@inyangeindustries.com</t>
+          <t>nbchvgmn@gmail.com</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>0788309662</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>www.inyangeindustries.com</t>
+          <t>0788475217</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>1197580006310064</t>
+          <t>1198380172943184</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Rwandan</t>
+          <t>RWANDA</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>NCBA</t>
+          <t>EQUITY BANK</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>100095380</t>
+          <t>103496546</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3102226900000M</t>
+          <t>3100989200000S</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BROADBAND SYSTEMS CORPORATION  LTD</t>
+          <t>H.VEDASTE COMPANY Ltd</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -762,27 +752,27 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>BROADBAND SYSTEMS CORPORATION  LTD</t>
+          <t>H.VEDASTE COMPANY Ltd</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
+          <t>Kicukiro/Kigali</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
+          <t>Kicukiro/Kigali</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
+          <t>Kicukiro/Kigali</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>7229 KIGALI, RWANDA</t>
+          <t>25 NGOMA</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -792,22 +782,17 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>gilbert.kayinamura@bsc.rw</t>
+          <t>hitimanaveda16@gmail.com</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>4141</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>www.bsc.rw</t>
+          <t>0788562686</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>1198080006094070</t>
+          <t>1196280064731068</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -817,24 +802,24 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>BK</t>
+          <t>BPR</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>101982714</t>
+          <t>115405774</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3114072400000X</t>
+          <t>3102226900000M</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CONNECT GLOBAL BUSINESS COMPANY Ltd</t>
+          <t>BROADBAND SYSTEMS CORPORATION  LTD</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -844,27 +829,27 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>CONNECT GLOBAL BUSINESS COMPANY Ltd</t>
+          <t>BROADBAND SYSTEMS CORPORATION  LTD</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>KIGALI - NYARUGENGE</t>
+          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>KIGALI - NYARUGENGE</t>
+          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>KIGALI - NYARUGENGE</t>
+          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>POB:5564 Kigali</t>
+          <t>7229 KIGALI, RWANDA</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -874,17 +859,22 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>niyafeos@yahoo.fr</t>
+          <t>gilbert.kayinamura@bsc.rw</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>788757320</t>
+          <t>4141</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>www.bsc.rw</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>1197980004514176</t>
+          <t>1198080006094070</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -894,12 +884,12 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>I&amp;M Bank</t>
+          <t>BK</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>106907027</t>
+          <t>101982714</t>
         </is>
       </c>
     </row>
@@ -988,12 +978,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>3109596400000L</t>
+          <t>3100960800000N</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>NEPOMSCENE BUSINESS COMPANY  LTD</t>
+          <t>INYANGE INDUSTRIES  LTD</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1003,22 +993,27 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>NEPOMSCENE BUSINESS COMPANY  LTD</t>
+          <t>INYANGE INDUSTRIES  LTD</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>NYAMAGABE District,Gasaka Sector</t>
+          <t>MASAKA GASABO DISTRICT</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>NYAMAGABE District,Gasaka Sector</t>
+          <t>MASAKA GASABO DISTRICT</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>NYAMAGABE District,Gasaka Sector</t>
+          <t>MASAKA GASABO DISTRICT</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>4584 kigali-rwanda</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1028,32 +1023,37 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>nbchvgmn@gmail.com</t>
+          <t>bjames@inyangeindustries.com</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>0788475217</t>
+          <t>0788309662</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>www.inyangeindustries.com</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>1198380172943184</t>
+          <t>1197580006310064</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>RWANDA</t>
+          <t>Rwandan</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>EQUITY BANK</t>
+          <t>NCBA</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>103496546</t>
+          <t>100095380</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Almost managing to serialize all the red flag computations as a scalability strategy
</commit_message>
<xml_diff>
--- a/data/cached_generated_reports/2024-2025/red_flag_10.xlsx
+++ b/data/cached_generated_reports/2024-2025/red_flag_10.xlsx
@@ -588,12 +588,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3100580400000V</t>
+          <t>3109596400000L</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SOCIETE RWANDAISE DES PNEUMATIQUES BANDAG  LTD</t>
+          <t>NEPOMSCENE BUSINESS COMPANY  LTD</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -603,27 +603,22 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>SOCIETE RWANDAISE DES PNEUMATIQUES BANDAG  LTD</t>
+          <t>NEPOMSCENE BUSINESS COMPANY  LTD</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Kicukiro- Rwanda</t>
+          <t>NYAMAGABE District,Gasaka Sector</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Kicukiro- Rwanda</t>
+          <t>NYAMAGABE District,Gasaka Sector</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Kicukiro- Rwanda</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>1132 kigali</t>
+          <t>NYAMAGABE District,Gasaka Sector</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -633,44 +628,44 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>bandag@subizo.com</t>
+          <t>nbchvgmn@gmail.com</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0788303361</t>
+          <t>0788475217</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>AA3035975</t>
+          <t>1198380172943184</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>ITALY</t>
+          <t>RWANDA</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>I&amp;M Bank</t>
+          <t>EQUITY BANK</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>100003368</t>
+          <t>103496546</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3109596400000L</t>
+          <t>3102226900000M</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>NEPOMSCENE BUSINESS COMPANY  LTD</t>
+          <t>BROADBAND SYSTEMS CORPORATION  LTD</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -680,22 +675,27 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>NEPOMSCENE BUSINESS COMPANY  LTD</t>
+          <t>BROADBAND SYSTEMS CORPORATION  LTD</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>NYAMAGABE District,Gasaka Sector</t>
+          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>NYAMAGABE District,Gasaka Sector</t>
+          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>NYAMAGABE District,Gasaka Sector</t>
+          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>7229 KIGALI, RWANDA</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -705,17 +705,22 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>nbchvgmn@gmail.com</t>
+          <t>gilbert.kayinamura@bsc.rw</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>0788475217</t>
+          <t>4141</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>www.bsc.rw</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>1198380172943184</t>
+          <t>1198080006094070</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -725,24 +730,24 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>EQUITY BANK</t>
+          <t>BK</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>103496546</t>
+          <t>101982714</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3100989200000S</t>
+          <t>3100580400000V</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>H.VEDASTE COMPANY Ltd</t>
+          <t>SOCIETE RWANDAISE DES PNEUMATIQUES BANDAG  LTD</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -752,27 +757,27 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>H.VEDASTE COMPANY Ltd</t>
+          <t>SOCIETE RWANDAISE DES PNEUMATIQUES BANDAG  LTD</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Kicukiro/Kigali</t>
+          <t>Kicukiro- Rwanda</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Kicukiro/Kigali</t>
+          <t>Kicukiro- Rwanda</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Kicukiro/Kigali</t>
+          <t>Kicukiro- Rwanda</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>25 NGOMA</t>
+          <t>1132 kigali</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -782,44 +787,44 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>hitimanaveda16@gmail.com</t>
+          <t>bandag@subizo.com</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0788562686</t>
+          <t>0788303361</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>1196280064731068</t>
+          <t>AA3035975</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>RWANDA</t>
+          <t>ITALY</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>BPR</t>
+          <t>I&amp;M Bank</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>115405774</t>
+          <t>100003368</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3102226900000M</t>
+          <t>3100989200000S</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BROADBAND SYSTEMS CORPORATION  LTD</t>
+          <t>H.VEDASTE COMPANY Ltd</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -829,27 +834,27 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>BROADBAND SYSTEMS CORPORATION  LTD</t>
+          <t>H.VEDASTE COMPANY Ltd</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
+          <t>Kicukiro/Kigali</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
+          <t>Kicukiro/Kigali</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Remera, Gisimenti Airport Road (kn5 Rda), Opposite ChezLando</t>
+          <t>Kicukiro/Kigali</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>7229 KIGALI, RWANDA</t>
+          <t>25 NGOMA</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -859,22 +864,17 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>gilbert.kayinamura@bsc.rw</t>
+          <t>hitimanaveda16@gmail.com</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>4141</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>www.bsc.rw</t>
+          <t>0788562686</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>1198080006094070</t>
+          <t>1196280064731068</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -884,12 +884,12 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>BK</t>
+          <t>BPR</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>101982714</t>
+          <t>115405774</t>
         </is>
       </c>
     </row>

</xml_diff>